<commit_message>
UPD: Añadir fase 2 - UML 4+1
</commit_message>
<xml_diff>
--- a/Fase 1/Evidencias Grupales/PLANILLA DE EVALUACIÓN FASE 1.xlsx
+++ b/Fase 1/Evidencias Grupales/PLANILLA DE EVALUACIÓN FASE 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://duoccl0-my.sharepoint.com/personal/ge_galan_profesor_duoc_cl/Documents/2024-2/Clases/CAPSTONE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Desktop\Repositorios\2024_2_PO_CAPSTONE_001D_GRUPO_7\Fase 1\Evidencias Grupales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="610" documentId="8_{2EFDF332-31E9-4C74-A6B5-E695634C1C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91B80DAC-7CE7-4715-8162-B9D290CDE525}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01519723-8A3E-47E6-B262-83143576F138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVALUACION1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
   <si>
     <t>PUNTOS</t>
   </si>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t>El desarrollo del plan de trabajo no permite determinar si el logro de los objetivos propuestos del proyecto son alcanzables en los tiempos para su desarrollo y no demuestran hitos claros para demostrar el estado de avance</t>
+  </si>
+  <si>
+    <t>Álvaro Arenas Cornejo</t>
   </si>
 </sst>
 </file>
@@ -1055,6 +1058,65 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1088,69 +1150,10 @@
     <xf numFmtId="0" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1485,7 +1488,7 @@
   <dimension ref="A2:K929"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -1509,7 +1512,7 @@
       <c r="D2" s="2">
         <v>0.25</v>
       </c>
-      <c r="E2" s="70">
+      <c r="E2" s="67">
         <v>1</v>
       </c>
     </row>
@@ -1523,13 +1526,15 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="57"/>
+      <c r="E3" s="54"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="38" t="s">
+        <v>95</v>
+      </c>
       <c r="C4" s="6">
         <f>EVALUACION1!$C$24</f>
         <v>7</v>
@@ -1538,7 +1543,7 @@
         <f>$C$35</f>
         <v>7</v>
       </c>
-      <c r="E4" s="82">
+      <c r="E4" s="51">
         <f>C4*C$2+D4*D$2</f>
         <v>7</v>
       </c>
@@ -1557,7 +1562,7 @@
         <f>C47</f>
         <v>7</v>
       </c>
-      <c r="E5" s="82">
+      <c r="E5" s="51">
         <f t="shared" ref="E5:E6" si="0">C5*C$2+D5*D$2</f>
         <v>7</v>
       </c>
@@ -1576,56 +1581,56 @@
         <f>C58</f>
         <v>7</v>
       </c>
-      <c r="E6" s="82">
+      <c r="E6" s="51">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="11" spans="1:11" ht="18" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="69" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="15"/>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="65" t="s">
+      <c r="D11" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="66"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="64"/>
     </row>
     <row r="12" spans="1:11" ht="14.4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="68"/>
+      <c r="A12" s="66"/>
       <c r="B12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="65" t="s">
+      <c r="C12" s="54"/>
+      <c r="D12" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="66"/>
-      <c r="F12" s="65" t="s">
+      <c r="E12" s="64"/>
+      <c r="F12" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="66"/>
-      <c r="H12" s="71" t="s">
+      <c r="G12" s="64"/>
+      <c r="H12" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="I12" s="66"/>
-      <c r="J12" s="65" t="s">
+      <c r="I12" s="64"/>
+      <c r="J12" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="66"/>
+      <c r="K12" s="64"/>
     </row>
     <row r="13" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="73"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="41" t="str">
         <f>RUBRICA!A5</f>
         <v>1. Describe brevemente en qué consiste el Proyecto APT, justificando su relevancia para el campo laboral de su carrera.</v>
@@ -1634,7 +1639,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="17" t="str">
-        <f t="shared" ref="D13:D17" si="1">IF($C13=CL,"X","")</f>
+        <f t="shared" ref="D13:D16" si="1">IF($C13=CL,"X","")</f>
         <v>X</v>
       </c>
       <c r="E13" s="17">
@@ -1642,7 +1647,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="17" t="str">
-        <f t="shared" ref="F13:F17" si="2">IF($C13=L,"X","")</f>
+        <f t="shared" ref="F13:F16" si="2">IF($C13=L,"X","")</f>
         <v/>
       </c>
       <c r="G13" s="17" t="str">
@@ -1650,7 +1655,7 @@
         <v/>
       </c>
       <c r="H13" s="17" t="str">
-        <f t="shared" ref="H13:H17" si="3">IF($C13=ML,"X","")</f>
+        <f t="shared" ref="H13:H16" si="3">IF($C13=ML,"X","")</f>
         <v/>
       </c>
       <c r="I13" s="17" t="str">
@@ -1658,16 +1663,16 @@
         <v/>
       </c>
       <c r="J13" s="17" t="str">
-        <f t="shared" ref="J13:J17" si="4">IF($C13=NL,"X","")</f>
+        <f t="shared" ref="J13:J16" si="4">IF($C13=NL,"X","")</f>
         <v/>
       </c>
       <c r="K13" s="17" t="str">
-        <f t="shared" ref="K13:K17" si="5">IF($J13="X",0,"")</f>
+        <f t="shared" ref="K13:K16" si="5">IF($J13="X",0,"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:11" ht="26.4" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="73"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="41" t="str">
         <f>RUBRICA!A6</f>
         <v>2. Relaciona el Proyecto APT con las competencias del perfil de egreso de su Plan de Estudio.</v>
@@ -1709,7 +1714,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="73"/>
+      <c r="A15" s="70"/>
       <c r="B15" s="41" t="str">
         <f>RUBRICA!A8</f>
         <v xml:space="preserve">4.  Argumenta por qué el proyecto es factible de realizarse en el marco de la asignatura. </v>
@@ -1751,7 +1756,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="14.4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="73"/>
+      <c r="A16" s="70"/>
       <c r="B16" s="41" t="str">
         <f>RUBRICA!A9</f>
         <v xml:space="preserve">5. Formula objetivos claros, concisos y coherentes con la disciplina y la situación a abordar. </v>
@@ -1793,7 +1798,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="73"/>
+      <c r="A17" s="70"/>
       <c r="B17" s="41" t="str">
         <f>RUBRICA!A10</f>
         <v>6. Propone una metodología de trabajo que permite alcanzar los objetivos propuestos y es pertinente con los requerimientos disciplinares.</v>
@@ -1802,40 +1807,40 @@
         <v>7</v>
       </c>
       <c r="D17" s="17" t="str">
-        <f>IF($C17=CL,"X","")</f>
+        <f t="shared" ref="D17:D22" si="12">IF($C17=CL,"X","")</f>
         <v>X</v>
       </c>
       <c r="E17" s="17">
-        <f t="shared" ref="E17" si="12">IF(D17="X",100*0.1,"")</f>
+        <f t="shared" ref="E17" si="13">IF(D17="X",100*0.1,"")</f>
         <v>10</v>
       </c>
       <c r="F17" s="17" t="str">
-        <f>IF($C17=L,"X","")</f>
+        <f t="shared" ref="F17:F22" si="14">IF($C17=L,"X","")</f>
         <v/>
       </c>
       <c r="G17" s="17" t="str">
-        <f t="shared" ref="G17" si="13">IF(F17="X",60*0.1,"")</f>
+        <f t="shared" ref="G17" si="15">IF(F17="X",60*0.1,"")</f>
         <v/>
       </c>
       <c r="H17" s="17" t="str">
-        <f>IF($C17=ML,"X","")</f>
+        <f t="shared" ref="H17:H22" si="16">IF($C17=ML,"X","")</f>
         <v/>
       </c>
       <c r="I17" s="17" t="str">
-        <f t="shared" ref="I17" si="14">IF(H17="X",30*0.1,"")</f>
+        <f t="shared" ref="I17" si="17">IF(H17="X",30*0.1,"")</f>
         <v/>
       </c>
       <c r="J17" s="17" t="str">
-        <f>IF($C17=NL,"X","")</f>
+        <f t="shared" ref="J17:J22" si="18">IF($C17=NL,"X","")</f>
         <v/>
       </c>
       <c r="K17" s="17" t="str">
-        <f t="shared" ref="K17:K22" si="15">IF($J17="X",0,"")</f>
+        <f t="shared" ref="K17:K22" si="19">IF($J17="X",0,"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="73"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="41" t="str">
         <f>RUBRICA!A11</f>
         <v xml:space="preserve">7. Establece un plan de trabajo para su proyecto APT considerando los recursos, duración, facilitadores y obstaculizadores en el desarrollo de las actividades. </v>
@@ -1844,40 +1849,40 @@
         <v>7</v>
       </c>
       <c r="D18" s="17" t="str">
-        <f>IF($C18=CL,"X","")</f>
+        <f t="shared" si="12"/>
         <v>X</v>
       </c>
       <c r="E18" s="17">
-        <f t="shared" ref="E18:E19" si="16">IF(D18="X",100*0.1,"")</f>
+        <f t="shared" ref="E18" si="20">IF(D18="X",100*0.1,"")</f>
         <v>10</v>
       </c>
       <c r="F18" s="17" t="str">
-        <f>IF($C18=L,"X","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G18" s="17" t="str">
-        <f t="shared" ref="G18:G19" si="17">IF(F18="X",60*0.1,"")</f>
+        <f t="shared" ref="G18" si="21">IF(F18="X",60*0.1,"")</f>
         <v/>
       </c>
       <c r="H18" s="17" t="str">
-        <f>IF($C18=ML,"X","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I18" s="17" t="str">
-        <f t="shared" ref="I18:I19" si="18">IF(H18="X",30*0.1,"")</f>
+        <f t="shared" ref="I18" si="22">IF(H18="X",30*0.1,"")</f>
         <v/>
       </c>
       <c r="J18" s="17" t="str">
-        <f>IF($C18=NL,"X","")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="K18" s="17" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="73"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="41" t="str">
         <f>RUBRICA!A12</f>
         <v>8. Determina evidencias, justificando cómo estas dan cuenta del logro de las actividades del Proyecto APT.</v>
@@ -1886,7 +1891,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="17" t="str">
-        <f>IF($C19=CL,"X","")</f>
+        <f t="shared" si="12"/>
         <v>X</v>
       </c>
       <c r="E19" s="17">
@@ -1894,32 +1899,32 @@
         <v>5</v>
       </c>
       <c r="F19" s="17" t="str">
-        <f>IF($C19=L,"X","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G19" s="17" t="str">
-        <f t="shared" ref="G19" si="19">IF(F19="X",60*0.05,"")</f>
+        <f t="shared" ref="G19" si="23">IF(F19="X",60*0.05,"")</f>
         <v/>
       </c>
       <c r="H19" s="17" t="str">
-        <f>IF($C19=ML,"X","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I19" s="17" t="str">
-        <f t="shared" ref="I19" si="20">IF(H19="X",30*0.05,"")</f>
+        <f t="shared" ref="I19" si="24">IF(H19="X",30*0.05,"")</f>
         <v/>
       </c>
       <c r="J19" s="17" t="str">
-        <f>IF($C19=NL,"X","")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="K19" s="17" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="73"/>
+      <c r="A20" s="70"/>
       <c r="B20" s="41" t="str">
         <f>RUBRICA!A13</f>
         <v xml:space="preserve">9. Utiliza reglas de redacción, ortografía (literal, puntual, acentual) y las normas para citas y referencias. </v>
@@ -1928,7 +1933,7 @@
         <v>7</v>
       </c>
       <c r="D20" s="17" t="str">
-        <f>IF($C20=CL,"X","")</f>
+        <f t="shared" si="12"/>
         <v>X</v>
       </c>
       <c r="E20" s="17">
@@ -1936,7 +1941,7 @@
         <v>5</v>
       </c>
       <c r="F20" s="17" t="str">
-        <f>IF($C20=L,"X","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G20" s="17" t="str">
@@ -1944,7 +1949,7 @@
         <v/>
       </c>
       <c r="H20" s="17" t="str">
-        <f>IF($C20=ML,"X","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I20" s="17" t="str">
@@ -1952,16 +1957,16 @@
         <v/>
       </c>
       <c r="J20" s="17" t="str">
-        <f>IF($C20=NL,"X","")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="K20" s="17" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:11" ht="22.8" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="73"/>
+      <c r="A21" s="70"/>
       <c r="B21" s="41" t="str">
         <f>RUBRICA!A14</f>
         <v>10. Cumple completando el contenido del informe de presentación del proyecto de acuerdo con la plantilla entregada.</v>
@@ -1970,7 +1975,7 @@
         <v>7</v>
       </c>
       <c r="D21" s="17" t="str">
-        <f>IF($C21=CL,"X","")</f>
+        <f t="shared" si="12"/>
         <v>X</v>
       </c>
       <c r="E21" s="17">
@@ -1978,7 +1983,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="17" t="str">
-        <f>IF($C21=L,"X","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G21" s="17" t="str">
@@ -1986,7 +1991,7 @@
         <v/>
       </c>
       <c r="H21" s="17" t="str">
-        <f>IF($C21=ML,"X","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I21" s="17" t="str">
@@ -1994,16 +1999,16 @@
         <v/>
       </c>
       <c r="J21" s="17" t="str">
-        <f>IF($C21=NL,"X","")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="K21" s="17" t="str">
-        <f t="shared" si="15"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="73"/>
+        <f t="shared" si="19"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="36" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="70"/>
       <c r="B22" s="41" t="str">
         <f>RUBRICA!A16</f>
         <v>12. Desarrolla un plan de trabajo que permita del logro de los objetivos propuestos del proyecto de 
@@ -2013,7 +2018,7 @@
         <v>7</v>
       </c>
       <c r="D22" s="17" t="str">
-        <f>IF($C22=CL,"X","")</f>
+        <f t="shared" si="12"/>
         <v>X</v>
       </c>
       <c r="E22" s="17">
@@ -2021,7 +2026,7 @@
         <v>10</v>
       </c>
       <c r="F22" s="17" t="str">
-        <f>IF($C22=L,"X","")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G22" s="17" t="str">
@@ -2029,7 +2034,7 @@
         <v/>
       </c>
       <c r="H22" s="17" t="str">
-        <f>IF($C22=ML,"X","")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I22" s="17" t="str">
@@ -2037,16 +2042,16 @@
         <v/>
       </c>
       <c r="J22" s="17" t="str">
-        <f>IF($C22=NL,"X","")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="K22" s="17" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="68"/>
+      <c r="A23" s="66"/>
       <c r="B23" s="40" t="s">
         <v>6</v>
       </c>
@@ -2076,7 +2081,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="57"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="43" t="s">
         <v>16</v>
       </c>
@@ -2088,82 +2093,82 @@
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="67" t="s">
+      <c r="A27" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="59">
+      <c r="C27" s="55" t="str">
         <f>$B$4</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="61"/>
+        <v>Álvaro Arenas Cornejo</v>
+      </c>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="57"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="68"/>
-      <c r="B28" s="57"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="63"/>
-      <c r="I28" s="63"/>
-      <c r="J28" s="63"/>
-      <c r="K28" s="64"/>
+      <c r="A28" s="66"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="59"/>
+      <c r="K28" s="60"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="68"/>
+      <c r="A29" s="66"/>
       <c r="B29" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="58" t="s">
+      <c r="C29" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="65" t="s">
+      <c r="D29" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="66"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="64"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="68"/>
+      <c r="A30" s="66"/>
       <c r="B30" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="65" t="s">
+      <c r="C30" s="54"/>
+      <c r="D30" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="65" t="s">
+      <c r="E30" s="64"/>
+      <c r="F30" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="66"/>
-      <c r="H30" s="65" t="s">
+      <c r="G30" s="64"/>
+      <c r="H30" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="I30" s="66"/>
-      <c r="J30" s="65" t="s">
+      <c r="I30" s="64"/>
+      <c r="J30" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="K30" s="66"/>
+      <c r="K30" s="64"/>
     </row>
     <row r="31" spans="1:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="68"/>
+      <c r="A31" s="66"/>
       <c r="B31" s="41" t="str">
         <f>RUBRICA!A7</f>
         <v>3. Relaciona el Proyecto APT con sus intereses profesionales. *</v>
@@ -2172,7 +2177,7 @@
         <v>7</v>
       </c>
       <c r="D31" s="17" t="str">
-        <f t="shared" ref="D31:D32" si="21">IF($C31=CL,"X","")</f>
+        <f t="shared" ref="D31:D32" si="25">IF($C31=CL,"X","")</f>
         <v>X</v>
       </c>
       <c r="E31" s="17">
@@ -2180,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="F31" s="17" t="str">
-        <f t="shared" ref="F31:F32" si="22">IF($C31=L,"X","")</f>
+        <f t="shared" ref="F31:F32" si="26">IF($C31=L,"X","")</f>
         <v/>
       </c>
       <c r="G31" s="17" t="str">
@@ -2188,7 +2193,7 @@
         <v/>
       </c>
       <c r="H31" s="17" t="str">
-        <f t="shared" ref="H31:H32" si="23">IF($C31=ML,"X","")</f>
+        <f t="shared" ref="H31:H32" si="27">IF($C31=ML,"X","")</f>
         <v/>
       </c>
       <c r="I31" s="17" t="str">
@@ -2196,16 +2201,16 @@
         <v/>
       </c>
       <c r="J31" s="17" t="str">
-        <f t="shared" ref="J31:J32" si="24">IF($C31=NL,"X","")</f>
+        <f t="shared" ref="J31:J32" si="28">IF($C31=NL,"X","")</f>
         <v/>
       </c>
       <c r="K31" s="17" t="str">
-        <f t="shared" ref="K31:K32" si="25">IF($J31="X",0,"")</f>
+        <f t="shared" ref="K31:K32" si="29">IF($J31="X",0,"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:11" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="68"/>
+      <c r="A32" s="66"/>
       <c r="B32" s="41" t="str">
         <f>RUBRICA!A15</f>
         <v>11. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</v>
@@ -2214,7 +2219,7 @@
         <v>7</v>
       </c>
       <c r="D32" s="17" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>X</v>
       </c>
       <c r="E32" s="17">
@@ -2222,7 +2227,7 @@
         <v>10</v>
       </c>
       <c r="F32" s="17" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="G32" s="17" t="str">
@@ -2230,7 +2235,7 @@
         <v/>
       </c>
       <c r="H32" s="17" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="I32" s="17" t="str">
@@ -2238,16 +2243,16 @@
         <v/>
       </c>
       <c r="J32" s="17" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="K32" s="17" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="68"/>
+      <c r="A33" s="66"/>
       <c r="B33" s="41" t="str">
         <f>RUBRICA!A17</f>
         <v>13. Colaboración y trabajo en equipo *</v>
@@ -2289,7 +2294,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="68"/>
+      <c r="A34" s="66"/>
       <c r="B34" s="22" t="s">
         <v>17</v>
       </c>
@@ -2304,22 +2309,22 @@
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="20">
-        <f t="shared" ref="G34:K34" si="26">SUM(G31:G33)</f>
+        <f t="shared" ref="G34:K34" si="30">SUM(G31:G33)</f>
         <v>0</v>
       </c>
       <c r="H34" s="20"/>
       <c r="I34" s="20">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="J34" s="20"/>
       <c r="K34" s="20">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="57"/>
+      <c r="A35" s="54"/>
       <c r="B35" s="18" t="s">
         <v>16</v>
       </c>
@@ -2338,82 +2343,82 @@
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="67" t="s">
+      <c r="A39" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="56" t="s">
+      <c r="B39" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="59">
+      <c r="C39" s="55">
         <f>B5</f>
         <v>0</v>
       </c>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="60"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="60"/>
-      <c r="K39" s="61"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="56"/>
+      <c r="J39" s="56"/>
+      <c r="K39" s="57"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="68"/>
-      <c r="B40" s="57"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="63"/>
-      <c r="F40" s="63"/>
-      <c r="G40" s="63"/>
-      <c r="H40" s="63"/>
-      <c r="I40" s="63"/>
-      <c r="J40" s="63"/>
-      <c r="K40" s="64"/>
+      <c r="A40" s="66"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="59"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="60"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="68"/>
+      <c r="A41" s="66"/>
       <c r="B41" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="58" t="s">
+      <c r="C41" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="65" t="s">
+      <c r="D41" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="E41" s="69"/>
-      <c r="F41" s="69"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="69"/>
-      <c r="I41" s="69"/>
-      <c r="J41" s="69"/>
-      <c r="K41" s="66"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
+      <c r="I41" s="63"/>
+      <c r="J41" s="63"/>
+      <c r="K41" s="64"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="68"/>
+      <c r="A42" s="66"/>
       <c r="B42" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="57"/>
-      <c r="D42" s="65" t="s">
+      <c r="C42" s="54"/>
+      <c r="D42" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="66"/>
-      <c r="F42" s="65" t="s">
+      <c r="E42" s="64"/>
+      <c r="F42" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="66"/>
-      <c r="H42" s="65" t="s">
+      <c r="G42" s="64"/>
+      <c r="H42" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="I42" s="66"/>
-      <c r="J42" s="65" t="s">
+      <c r="I42" s="64"/>
+      <c r="J42" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="K42" s="66"/>
+      <c r="K42" s="64"/>
     </row>
     <row r="43" spans="1:11" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="68"/>
+      <c r="A43" s="66"/>
       <c r="B43" s="41" t="str">
         <f>RUBRICA!A7</f>
         <v>3. Relaciona el Proyecto APT con sus intereses profesionales. *</v>
@@ -2422,7 +2427,7 @@
         <v>7</v>
       </c>
       <c r="D43" s="17" t="str">
-        <f t="shared" ref="D43:D44" si="27">IF($C43=CL,"X","")</f>
+        <f t="shared" ref="D43:D44" si="31">IF($C43=CL,"X","")</f>
         <v>X</v>
       </c>
       <c r="E43" s="17">
@@ -2430,7 +2435,7 @@
         <v>10</v>
       </c>
       <c r="F43" s="17" t="str">
-        <f t="shared" ref="F43:F44" si="28">IF($C43=L,"X","")</f>
+        <f t="shared" ref="F43:F44" si="32">IF($C43=L,"X","")</f>
         <v/>
       </c>
       <c r="G43" s="17" t="str">
@@ -2438,7 +2443,7 @@
         <v/>
       </c>
       <c r="H43" s="17" t="str">
-        <f t="shared" ref="H43:H44" si="29">IF($C43=ML,"X","")</f>
+        <f t="shared" ref="H43:H44" si="33">IF($C43=ML,"X","")</f>
         <v/>
       </c>
       <c r="I43" s="17" t="str">
@@ -2446,16 +2451,16 @@
         <v/>
       </c>
       <c r="J43" s="17" t="str">
-        <f t="shared" ref="J43:J44" si="30">IF($C43=NL,"X","")</f>
+        <f t="shared" ref="J43:J44" si="34">IF($C43=NL,"X","")</f>
         <v/>
       </c>
       <c r="K43" s="17" t="str">
-        <f t="shared" ref="K43:K44" si="31">IF($J43="X",0,"")</f>
+        <f t="shared" ref="K43:K44" si="35">IF($J43="X",0,"")</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:11" ht="24" x14ac:dyDescent="0.3">
-      <c r="A44" s="68"/>
+      <c r="A44" s="66"/>
       <c r="B44" s="41" t="str">
         <f>RUBRICA!A15</f>
         <v>11. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</v>
@@ -2464,7 +2469,7 @@
         <v>7</v>
       </c>
       <c r="D44" s="17" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>X</v>
       </c>
       <c r="E44" s="17">
@@ -2472,7 +2477,7 @@
         <v>10</v>
       </c>
       <c r="F44" s="17" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="G44" s="17" t="str">
@@ -2480,7 +2485,7 @@
         <v/>
       </c>
       <c r="H44" s="17" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="I44" s="17" t="str">
@@ -2488,16 +2493,16 @@
         <v/>
       </c>
       <c r="J44" s="17" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="K44" s="17" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="68"/>
+      <c r="A45" s="66"/>
       <c r="B45" s="41" t="str">
         <f>RUBRICA!A17</f>
         <v>13. Colaboración y trabajo en equipo *</v>
@@ -2539,7 +2544,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="68"/>
+      <c r="A46" s="66"/>
       <c r="B46" s="22" t="s">
         <v>17</v>
       </c>
@@ -2554,22 +2559,22 @@
       </c>
       <c r="F46" s="20"/>
       <c r="G46" s="20">
-        <f t="shared" ref="G46" si="32">SUM(G43:G45)</f>
+        <f t="shared" ref="G46" si="36">SUM(G43:G45)</f>
         <v>0</v>
       </c>
       <c r="H46" s="20"/>
       <c r="I46" s="20">
-        <f t="shared" ref="I46" si="33">SUM(I43:I45)</f>
+        <f t="shared" ref="I46" si="37">SUM(I43:I45)</f>
         <v>0</v>
       </c>
       <c r="J46" s="20"/>
       <c r="K46" s="20">
-        <f t="shared" ref="K46" si="34">SUM(K43:K45)</f>
+        <f t="shared" ref="K46" si="38">SUM(K43:K45)</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="57"/>
+      <c r="A47" s="54"/>
       <c r="B47" s="18" t="s">
         <v>16</v>
       </c>
@@ -2587,82 +2592,82 @@
       <c r="C49" s="24"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="67" t="s">
+      <c r="A50" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="B50" s="56" t="s">
+      <c r="B50" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="59">
+      <c r="C50" s="55">
         <f>B6</f>
         <v>0</v>
       </c>
-      <c r="D50" s="60"/>
-      <c r="E50" s="60"/>
-      <c r="F50" s="60"/>
-      <c r="G50" s="60"/>
-      <c r="H50" s="60"/>
-      <c r="I50" s="60"/>
-      <c r="J50" s="60"/>
-      <c r="K50" s="61"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="56"/>
+      <c r="H50" s="56"/>
+      <c r="I50" s="56"/>
+      <c r="J50" s="56"/>
+      <c r="K50" s="57"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="68"/>
-      <c r="B51" s="57"/>
-      <c r="C51" s="62"/>
-      <c r="D51" s="63"/>
-      <c r="E51" s="63"/>
-      <c r="F51" s="63"/>
-      <c r="G51" s="63"/>
-      <c r="H51" s="63"/>
-      <c r="I51" s="63"/>
-      <c r="J51" s="63"/>
-      <c r="K51" s="64"/>
+      <c r="A51" s="66"/>
+      <c r="B51" s="54"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="59"/>
+      <c r="G51" s="59"/>
+      <c r="H51" s="59"/>
+      <c r="I51" s="59"/>
+      <c r="J51" s="59"/>
+      <c r="K51" s="60"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="68"/>
+      <c r="A52" s="66"/>
       <c r="B52" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="58" t="s">
+      <c r="C52" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D52" s="65" t="s">
+      <c r="D52" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="69"/>
-      <c r="F52" s="69"/>
-      <c r="G52" s="69"/>
-      <c r="H52" s="69"/>
-      <c r="I52" s="69"/>
-      <c r="J52" s="69"/>
-      <c r="K52" s="66"/>
+      <c r="E52" s="63"/>
+      <c r="F52" s="63"/>
+      <c r="G52" s="63"/>
+      <c r="H52" s="63"/>
+      <c r="I52" s="63"/>
+      <c r="J52" s="63"/>
+      <c r="K52" s="64"/>
     </row>
     <row r="53" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="68"/>
+      <c r="A53" s="66"/>
       <c r="B53" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="57"/>
-      <c r="D53" s="65" t="s">
+      <c r="C53" s="54"/>
+      <c r="D53" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="E53" s="66"/>
-      <c r="F53" s="65" t="s">
+      <c r="E53" s="64"/>
+      <c r="F53" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="G53" s="66"/>
-      <c r="H53" s="65" t="s">
+      <c r="G53" s="64"/>
+      <c r="H53" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="I53" s="66"/>
-      <c r="J53" s="65" t="s">
+      <c r="I53" s="64"/>
+      <c r="J53" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="K53" s="66"/>
+      <c r="K53" s="64"/>
     </row>
     <row r="54" spans="1:11" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="68"/>
+      <c r="A54" s="66"/>
       <c r="B54" s="41" t="str">
         <f>RUBRICA!A7</f>
         <v>3. Relaciona el Proyecto APT con sus intereses profesionales. *</v>
@@ -2671,7 +2676,7 @@
         <v>7</v>
       </c>
       <c r="D54" s="17" t="str">
-        <f t="shared" ref="D54:D55" si="35">IF($C54=CL,"X","")</f>
+        <f t="shared" ref="D54:D55" si="39">IF($C54=CL,"X","")</f>
         <v>X</v>
       </c>
       <c r="E54" s="17">
@@ -2679,7 +2684,7 @@
         <v>10</v>
       </c>
       <c r="F54" s="17" t="str">
-        <f t="shared" ref="F54:F55" si="36">IF($C54=L,"X","")</f>
+        <f t="shared" ref="F54:F55" si="40">IF($C54=L,"X","")</f>
         <v/>
       </c>
       <c r="G54" s="17" t="str">
@@ -2687,7 +2692,7 @@
         <v/>
       </c>
       <c r="H54" s="17" t="str">
-        <f t="shared" ref="H54:H55" si="37">IF($C54=ML,"X","")</f>
+        <f t="shared" ref="H54:H55" si="41">IF($C54=ML,"X","")</f>
         <v/>
       </c>
       <c r="I54" s="17" t="str">
@@ -2695,16 +2700,16 @@
         <v/>
       </c>
       <c r="J54" s="17" t="str">
-        <f t="shared" ref="J54:J55" si="38">IF($C54=NL,"X","")</f>
+        <f t="shared" ref="J54:J55" si="42">IF($C54=NL,"X","")</f>
         <v/>
       </c>
       <c r="K54" s="17" t="str">
-        <f t="shared" ref="K54:K55" si="39">IF($J54="X",0,"")</f>
+        <f t="shared" ref="K54:K55" si="43">IF($J54="X",0,"")</f>
         <v/>
       </c>
     </row>
     <row r="55" spans="1:11" ht="24" x14ac:dyDescent="0.3">
-      <c r="A55" s="68"/>
+      <c r="A55" s="66"/>
       <c r="B55" s="41" t="str">
         <f>RUBRICA!A15</f>
         <v>11. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</v>
@@ -2713,7 +2718,7 @@
         <v>7</v>
       </c>
       <c r="D55" s="17" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>X</v>
       </c>
       <c r="E55" s="17">
@@ -2721,7 +2726,7 @@
         <v>10</v>
       </c>
       <c r="F55" s="17" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="G55" s="17" t="str">
@@ -2729,7 +2734,7 @@
         <v/>
       </c>
       <c r="H55" s="17" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="I55" s="17" t="str">
@@ -2737,16 +2742,16 @@
         <v/>
       </c>
       <c r="J55" s="17" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="K55" s="17" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="68"/>
+      <c r="A56" s="66"/>
       <c r="B56" s="41" t="str">
         <f>RUBRICA!A17</f>
         <v>13. Colaboración y trabajo en equipo *</v>
@@ -2788,7 +2793,7 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="68"/>
+      <c r="A57" s="66"/>
       <c r="B57" s="22" t="s">
         <v>17</v>
       </c>
@@ -2805,32 +2810,32 @@
         <v>30</v>
       </c>
       <c r="F57" s="20">
-        <f t="shared" ref="F57" si="40">SUM(F54:F56)</f>
+        <f t="shared" ref="F57" si="44">SUM(F54:F56)</f>
         <v>0</v>
       </c>
       <c r="G57" s="20">
-        <f t="shared" ref="G57" si="41">SUM(G54:G56)</f>
+        <f t="shared" ref="G57" si="45">SUM(G54:G56)</f>
         <v>0</v>
       </c>
       <c r="H57" s="20">
-        <f t="shared" ref="H57" si="42">SUM(H54:H56)</f>
+        <f t="shared" ref="H57" si="46">SUM(H54:H56)</f>
         <v>0</v>
       </c>
       <c r="I57" s="20">
-        <f t="shared" ref="I57" si="43">SUM(I54:I56)</f>
+        <f t="shared" ref="I57" si="47">SUM(I54:I56)</f>
         <v>0</v>
       </c>
       <c r="J57" s="20">
-        <f t="shared" ref="J57" si="44">SUM(J54:J56)</f>
+        <f t="shared" ref="J57" si="48">SUM(J54:J56)</f>
         <v>0</v>
       </c>
       <c r="K57" s="20">
-        <f t="shared" ref="K57" si="45">SUM(K54:K56)</f>
+        <f t="shared" ref="K57" si="49">SUM(K54:K56)</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="57"/>
+      <c r="A58" s="54"/>
       <c r="B58" s="18" t="s">
         <v>16</v>
       </c>
@@ -3715,14 +3720,17 @@
     <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:K40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:K41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C50:K51"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="A50:A58"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="D52:K52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:I53"/>
     <mergeCell ref="A39:A47"/>
     <mergeCell ref="A27:A35"/>
     <mergeCell ref="E2:E3"/>
@@ -3739,17 +3747,14 @@
     <mergeCell ref="D29:K29"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="D52:K52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C50:K51"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="A50:A58"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:K40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:K41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:E6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
@@ -3801,25 +3806,25 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="48" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="74" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="49"/>
-      <c r="B3" s="54" t="s">
+      <c r="A3" s="75"/>
+      <c r="B3" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="80" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="26" t="s">
@@ -3828,19 +3833,19 @@
       <c r="E3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="49"/>
+      <c r="F3" s="75"/>
     </row>
     <row r="4" spans="1:6" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="50"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
+      <c r="A4" s="76"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
       <c r="D4" s="27">
         <v>-0.3</v>
       </c>
       <c r="E4" s="27">
         <v>0</v>
       </c>
-      <c r="F4" s="50"/>
+      <c r="F4" s="76"/>
     </row>
     <row r="5" spans="1:6" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
@@ -3983,7 +3988,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="47" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="32" t="s">
@@ -3998,7 +4003,7 @@
       <c r="E12" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="79">
+      <c r="F12" s="48">
         <v>5</v>
       </c>
     </row>
@@ -4018,27 +4023,27 @@
       <c r="E13" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="80">
+      <c r="F13" s="49">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="69" x14ac:dyDescent="0.3">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="81" t="s">
+      <c r="C14" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="81" t="s">
+      <c r="D14" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="81" t="s">
+      <c r="E14" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="80">
+      <c r="F14" s="49">
         <v>5</v>
       </c>
     </row>
@@ -4046,7 +4051,7 @@
       <c r="A15" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="46" t="s">
         <v>79</v>
       </c>
       <c r="C15" s="30" t="s">
@@ -4063,19 +4068,19 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="76" t="s">
+      <c r="A16" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="77" t="s">
+      <c r="B16" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="77" t="s">
+      <c r="C16" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="77" t="s">
+      <c r="D16" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="E16" s="77" t="s">
+      <c r="E16" s="46" t="s">
         <v>94</v>
       </c>
       <c r="F16" s="31">
@@ -4103,13 +4108,13 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="47"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="73"/>
       <c r="F18" s="33">
         <v>1</v>
       </c>
@@ -4152,7 +4157,7 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="83">
+      <c r="B2" s="52">
         <v>1</v>
       </c>
     </row>
@@ -4160,7 +4165,7 @@
       <c r="A3">
         <v>0.5</v>
       </c>
-      <c r="B3" s="83">
+      <c r="B3" s="52">
         <v>1</v>
       </c>
     </row>
@@ -4168,7 +4173,7 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="83">
+      <c r="B4" s="52">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -4176,7 +4181,7 @@
       <c r="A5">
         <v>1.5</v>
       </c>
-      <c r="B5" s="83">
+      <c r="B5" s="52">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -4184,7 +4189,7 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="83">
+      <c r="B6" s="52">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -4192,7 +4197,7 @@
       <c r="A7">
         <v>2.5</v>
       </c>
-      <c r="B7" s="83">
+      <c r="B7" s="52">
         <v>1.2</v>
       </c>
     </row>
@@ -4200,7 +4205,7 @@
       <c r="A8">
         <v>3</v>
       </c>
-      <c r="B8" s="83">
+      <c r="B8" s="52">
         <v>1.2</v>
       </c>
     </row>
@@ -4208,7 +4213,7 @@
       <c r="A9">
         <v>3.5</v>
       </c>
-      <c r="B9" s="83">
+      <c r="B9" s="52">
         <v>1.3</v>
       </c>
     </row>
@@ -4216,7 +4221,7 @@
       <c r="A10">
         <v>4</v>
       </c>
-      <c r="B10" s="83">
+      <c r="B10" s="52">
         <v>1.3</v>
       </c>
     </row>
@@ -4224,7 +4229,7 @@
       <c r="A11">
         <v>4.5</v>
       </c>
-      <c r="B11" s="83">
+      <c r="B11" s="52">
         <v>1.3</v>
       </c>
     </row>
@@ -4232,7 +4237,7 @@
       <c r="A12">
         <v>5</v>
       </c>
-      <c r="B12" s="83">
+      <c r="B12" s="52">
         <v>1.4</v>
       </c>
     </row>
@@ -4240,7 +4245,7 @@
       <c r="A13">
         <v>5.5</v>
       </c>
-      <c r="B13" s="83">
+      <c r="B13" s="52">
         <v>1.4</v>
       </c>
     </row>
@@ -4248,7 +4253,7 @@
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" s="83">
+      <c r="B14" s="52">
         <v>1.4</v>
       </c>
     </row>
@@ -4256,7 +4261,7 @@
       <c r="A15">
         <v>6.5</v>
       </c>
-      <c r="B15" s="83">
+      <c r="B15" s="52">
         <v>1.5</v>
       </c>
     </row>
@@ -4264,7 +4269,7 @@
       <c r="A16">
         <v>7</v>
       </c>
-      <c r="B16" s="83">
+      <c r="B16" s="52">
         <v>1.5</v>
       </c>
     </row>
@@ -4272,7 +4277,7 @@
       <c r="A17">
         <v>7.5</v>
       </c>
-      <c r="B17" s="83">
+      <c r="B17" s="52">
         <v>1.5</v>
       </c>
     </row>
@@ -4280,7 +4285,7 @@
       <c r="A18">
         <v>8</v>
       </c>
-      <c r="B18" s="83">
+      <c r="B18" s="52">
         <v>1.6</v>
       </c>
     </row>
@@ -4288,7 +4293,7 @@
       <c r="A19">
         <v>8.5</v>
       </c>
-      <c r="B19" s="83">
+      <c r="B19" s="52">
         <v>1.6</v>
       </c>
     </row>
@@ -4296,7 +4301,7 @@
       <c r="A20">
         <v>9</v>
       </c>
-      <c r="B20" s="83">
+      <c r="B20" s="52">
         <v>1.6</v>
       </c>
     </row>
@@ -4304,7 +4309,7 @@
       <c r="A21">
         <v>9.5</v>
       </c>
-      <c r="B21" s="83">
+      <c r="B21" s="52">
         <v>1.7</v>
       </c>
     </row>
@@ -4312,7 +4317,7 @@
       <c r="A22">
         <v>10</v>
       </c>
-      <c r="B22" s="83">
+      <c r="B22" s="52">
         <v>1.7</v>
       </c>
     </row>
@@ -4320,7 +4325,7 @@
       <c r="A23">
         <v>10.5</v>
       </c>
-      <c r="B23" s="83">
+      <c r="B23" s="52">
         <v>1.8</v>
       </c>
     </row>
@@ -4328,7 +4333,7 @@
       <c r="A24">
         <v>11</v>
       </c>
-      <c r="B24" s="83">
+      <c r="B24" s="52">
         <v>1.8</v>
       </c>
     </row>
@@ -4336,7 +4341,7 @@
       <c r="A25">
         <v>11.5</v>
       </c>
-      <c r="B25" s="83">
+      <c r="B25" s="52">
         <v>1.8</v>
       </c>
     </row>
@@ -4344,7 +4349,7 @@
       <c r="A26">
         <v>12</v>
       </c>
-      <c r="B26" s="83">
+      <c r="B26" s="52">
         <v>1.9</v>
       </c>
     </row>
@@ -4352,7 +4357,7 @@
       <c r="A27">
         <v>12.5</v>
       </c>
-      <c r="B27" s="83">
+      <c r="B27" s="52">
         <v>1.9</v>
       </c>
     </row>
@@ -4360,7 +4365,7 @@
       <c r="A28">
         <v>13</v>
       </c>
-      <c r="B28" s="83">
+      <c r="B28" s="52">
         <v>1.9</v>
       </c>
     </row>
@@ -4368,7 +4373,7 @@
       <c r="A29">
         <v>13.5</v>
       </c>
-      <c r="B29" s="83">
+      <c r="B29" s="52">
         <v>2</v>
       </c>
     </row>
@@ -4376,7 +4381,7 @@
       <c r="A30">
         <v>14</v>
       </c>
-      <c r="B30" s="83">
+      <c r="B30" s="52">
         <v>2</v>
       </c>
     </row>
@@ -4384,7 +4389,7 @@
       <c r="A31">
         <v>14.5</v>
       </c>
-      <c r="B31" s="83">
+      <c r="B31" s="52">
         <v>2</v>
       </c>
     </row>
@@ -4392,7 +4397,7 @@
       <c r="A32">
         <v>15</v>
       </c>
-      <c r="B32" s="83">
+      <c r="B32" s="52">
         <v>2.1</v>
       </c>
     </row>
@@ -4400,7 +4405,7 @@
       <c r="A33">
         <v>15.5</v>
       </c>
-      <c r="B33" s="83">
+      <c r="B33" s="52">
         <v>2.1</v>
       </c>
     </row>
@@ -4408,7 +4413,7 @@
       <c r="A34">
         <v>16</v>
       </c>
-      <c r="B34" s="83">
+      <c r="B34" s="52">
         <v>2.1</v>
       </c>
     </row>
@@ -4416,7 +4421,7 @@
       <c r="A35">
         <v>16.5</v>
       </c>
-      <c r="B35" s="83">
+      <c r="B35" s="52">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -4424,7 +4429,7 @@
       <c r="A36">
         <v>17</v>
       </c>
-      <c r="B36" s="83">
+      <c r="B36" s="52">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -4432,7 +4437,7 @@
       <c r="A37">
         <v>17.5</v>
       </c>
-      <c r="B37" s="83">
+      <c r="B37" s="52">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -4440,7 +4445,7 @@
       <c r="A38">
         <v>18</v>
       </c>
-      <c r="B38" s="83">
+      <c r="B38" s="52">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -4448,7 +4453,7 @@
       <c r="A39">
         <v>18.5</v>
       </c>
-      <c r="B39" s="83">
+      <c r="B39" s="52">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -4456,7 +4461,7 @@
       <c r="A40">
         <v>19</v>
       </c>
-      <c r="B40" s="83">
+      <c r="B40" s="52">
         <v>2.4</v>
       </c>
     </row>
@@ -4464,7 +4469,7 @@
       <c r="A41">
         <v>19.5</v>
       </c>
-      <c r="B41" s="83">
+      <c r="B41" s="52">
         <v>2.4</v>
       </c>
     </row>
@@ -4472,7 +4477,7 @@
       <c r="A42">
         <v>20</v>
       </c>
-      <c r="B42" s="83">
+      <c r="B42" s="52">
         <v>2.4</v>
       </c>
     </row>
@@ -4480,7 +4485,7 @@
       <c r="A43">
         <v>20.5</v>
       </c>
-      <c r="B43" s="83">
+      <c r="B43" s="52">
         <v>2.5</v>
       </c>
     </row>
@@ -4488,7 +4493,7 @@
       <c r="A44">
         <v>21</v>
       </c>
-      <c r="B44" s="83">
+      <c r="B44" s="52">
         <v>2.5</v>
       </c>
     </row>
@@ -4496,7 +4501,7 @@
       <c r="A45">
         <v>21.5</v>
       </c>
-      <c r="B45" s="83">
+      <c r="B45" s="52">
         <v>2.5</v>
       </c>
     </row>
@@ -4504,7 +4509,7 @@
       <c r="A46">
         <v>22</v>
       </c>
-      <c r="B46" s="83">
+      <c r="B46" s="52">
         <v>2.6</v>
       </c>
     </row>
@@ -4512,7 +4517,7 @@
       <c r="A47">
         <v>22.5</v>
       </c>
-      <c r="B47" s="83">
+      <c r="B47" s="52">
         <v>2.6</v>
       </c>
     </row>
@@ -4520,7 +4525,7 @@
       <c r="A48">
         <v>23</v>
       </c>
-      <c r="B48" s="83">
+      <c r="B48" s="52">
         <v>2.6</v>
       </c>
     </row>
@@ -4528,7 +4533,7 @@
       <c r="A49">
         <v>23.5</v>
       </c>
-      <c r="B49" s="83">
+      <c r="B49" s="52">
         <v>2.7</v>
       </c>
     </row>
@@ -4536,7 +4541,7 @@
       <c r="A50">
         <v>24</v>
       </c>
-      <c r="B50" s="83">
+      <c r="B50" s="52">
         <v>2.7</v>
       </c>
     </row>
@@ -4544,7 +4549,7 @@
       <c r="A51">
         <v>24.5</v>
       </c>
-      <c r="B51" s="83">
+      <c r="B51" s="52">
         <v>2.8</v>
       </c>
     </row>
@@ -4552,7 +4557,7 @@
       <c r="A52">
         <v>25</v>
       </c>
-      <c r="B52" s="83">
+      <c r="B52" s="52">
         <v>2.8</v>
       </c>
     </row>
@@ -4560,7 +4565,7 @@
       <c r="A53">
         <v>25.5</v>
       </c>
-      <c r="B53" s="83">
+      <c r="B53" s="52">
         <v>2.8</v>
       </c>
     </row>
@@ -4568,7 +4573,7 @@
       <c r="A54">
         <v>26</v>
       </c>
-      <c r="B54" s="83">
+      <c r="B54" s="52">
         <v>2.9</v>
       </c>
     </row>
@@ -4576,7 +4581,7 @@
       <c r="A55">
         <v>26.5</v>
       </c>
-      <c r="B55" s="83">
+      <c r="B55" s="52">
         <v>2.9</v>
       </c>
     </row>
@@ -4584,7 +4589,7 @@
       <c r="A56">
         <v>27</v>
       </c>
-      <c r="B56" s="83">
+      <c r="B56" s="52">
         <v>2.9</v>
       </c>
     </row>
@@ -4592,7 +4597,7 @@
       <c r="A57">
         <v>27.5</v>
       </c>
-      <c r="B57" s="83">
+      <c r="B57" s="52">
         <v>3</v>
       </c>
     </row>
@@ -4600,7 +4605,7 @@
       <c r="A58">
         <v>28</v>
       </c>
-      <c r="B58" s="83">
+      <c r="B58" s="52">
         <v>3</v>
       </c>
     </row>
@@ -4608,7 +4613,7 @@
       <c r="A59">
         <v>28.5</v>
       </c>
-      <c r="B59" s="83">
+      <c r="B59" s="52">
         <v>3</v>
       </c>
     </row>
@@ -4616,7 +4621,7 @@
       <c r="A60">
         <v>29</v>
       </c>
-      <c r="B60" s="83">
+      <c r="B60" s="52">
         <v>3.1</v>
       </c>
     </row>
@@ -4624,7 +4629,7 @@
       <c r="A61">
         <v>29.5</v>
       </c>
-      <c r="B61" s="83">
+      <c r="B61" s="52">
         <v>3.1</v>
       </c>
     </row>
@@ -4632,7 +4637,7 @@
       <c r="A62">
         <v>30</v>
       </c>
-      <c r="B62" s="83">
+      <c r="B62" s="52">
         <v>3.1</v>
       </c>
     </row>
@@ -4640,7 +4645,7 @@
       <c r="A63">
         <v>30.5</v>
       </c>
-      <c r="B63" s="83">
+      <c r="B63" s="52">
         <v>3.2</v>
       </c>
     </row>
@@ -4648,7 +4653,7 @@
       <c r="A64">
         <v>31</v>
       </c>
-      <c r="B64" s="83">
+      <c r="B64" s="52">
         <v>3.2</v>
       </c>
     </row>
@@ -4656,7 +4661,7 @@
       <c r="A65">
         <v>31.5</v>
       </c>
-      <c r="B65" s="83">
+      <c r="B65" s="52">
         <v>3.3</v>
       </c>
     </row>
@@ -4664,7 +4669,7 @@
       <c r="A66">
         <v>32</v>
       </c>
-      <c r="B66" s="83">
+      <c r="B66" s="52">
         <v>3.3</v>
       </c>
     </row>
@@ -4672,7 +4677,7 @@
       <c r="A67">
         <v>32.5</v>
       </c>
-      <c r="B67" s="83">
+      <c r="B67" s="52">
         <v>3.3</v>
       </c>
     </row>
@@ -4680,7 +4685,7 @@
       <c r="A68">
         <v>33</v>
       </c>
-      <c r="B68" s="83">
+      <c r="B68" s="52">
         <v>3.4</v>
       </c>
     </row>
@@ -4688,7 +4693,7 @@
       <c r="A69">
         <v>33.5</v>
       </c>
-      <c r="B69" s="83">
+      <c r="B69" s="52">
         <v>3.4</v>
       </c>
     </row>
@@ -4696,7 +4701,7 @@
       <c r="A70">
         <v>34</v>
       </c>
-      <c r="B70" s="83">
+      <c r="B70" s="52">
         <v>3.4</v>
       </c>
     </row>
@@ -4704,7 +4709,7 @@
       <c r="A71">
         <v>34.5</v>
       </c>
-      <c r="B71" s="83">
+      <c r="B71" s="52">
         <v>3.5</v>
       </c>
     </row>
@@ -4712,7 +4717,7 @@
       <c r="A72">
         <v>35</v>
       </c>
-      <c r="B72" s="83">
+      <c r="B72" s="52">
         <v>3.5</v>
       </c>
     </row>
@@ -4720,7 +4725,7 @@
       <c r="A73">
         <v>35.5</v>
       </c>
-      <c r="B73" s="83">
+      <c r="B73" s="52">
         <v>3.5</v>
       </c>
     </row>
@@ -4728,7 +4733,7 @@
       <c r="A74">
         <v>36</v>
       </c>
-      <c r="B74" s="83">
+      <c r="B74" s="52">
         <v>3.6</v>
       </c>
     </row>
@@ -4736,7 +4741,7 @@
       <c r="A75">
         <v>36.5</v>
       </c>
-      <c r="B75" s="83">
+      <c r="B75" s="52">
         <v>3.6</v>
       </c>
     </row>
@@ -4744,7 +4749,7 @@
       <c r="A76">
         <v>37</v>
       </c>
-      <c r="B76" s="83">
+      <c r="B76" s="52">
         <v>3.6</v>
       </c>
     </row>
@@ -4752,7 +4757,7 @@
       <c r="A77">
         <v>37.5</v>
       </c>
-      <c r="B77" s="83">
+      <c r="B77" s="52">
         <v>3.7</v>
       </c>
     </row>
@@ -4760,7 +4765,7 @@
       <c r="A78">
         <v>38</v>
       </c>
-      <c r="B78" s="83">
+      <c r="B78" s="52">
         <v>3.7</v>
       </c>
     </row>
@@ -4768,7 +4773,7 @@
       <c r="A79">
         <v>38.5</v>
       </c>
-      <c r="B79" s="83">
+      <c r="B79" s="52">
         <v>3.8</v>
       </c>
     </row>
@@ -4776,7 +4781,7 @@
       <c r="A80">
         <v>39</v>
       </c>
-      <c r="B80" s="83">
+      <c r="B80" s="52">
         <v>3.8</v>
       </c>
     </row>
@@ -4784,7 +4789,7 @@
       <c r="A81">
         <v>39.5</v>
       </c>
-      <c r="B81" s="83">
+      <c r="B81" s="52">
         <v>3.8</v>
       </c>
     </row>
@@ -4792,7 +4797,7 @@
       <c r="A82">
         <v>40</v>
       </c>
-      <c r="B82" s="83">
+      <c r="B82" s="52">
         <v>3.9</v>
       </c>
     </row>
@@ -4800,7 +4805,7 @@
       <c r="A83">
         <v>40.5</v>
       </c>
-      <c r="B83" s="83">
+      <c r="B83" s="52">
         <v>3.9</v>
       </c>
     </row>
@@ -4808,7 +4813,7 @@
       <c r="A84">
         <v>41</v>
       </c>
-      <c r="B84" s="83">
+      <c r="B84" s="52">
         <v>3.9</v>
       </c>
     </row>
@@ -4816,7 +4821,7 @@
       <c r="A85">
         <v>41.5</v>
       </c>
-      <c r="B85" s="83">
+      <c r="B85" s="52">
         <v>4</v>
       </c>
     </row>
@@ -4824,7 +4829,7 @@
       <c r="A86">
         <v>42</v>
       </c>
-      <c r="B86" s="83">
+      <c r="B86" s="52">
         <v>4</v>
       </c>
     </row>
@@ -4832,7 +4837,7 @@
       <c r="A87">
         <v>42.5</v>
       </c>
-      <c r="B87" s="83">
+      <c r="B87" s="52">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -4840,7 +4845,7 @@
       <c r="A88">
         <v>43</v>
       </c>
-      <c r="B88" s="83">
+      <c r="B88" s="52">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -4848,7 +4853,7 @@
       <c r="A89">
         <v>43.5</v>
       </c>
-      <c r="B89" s="83">
+      <c r="B89" s="52">
         <v>4.2</v>
       </c>
     </row>
@@ -4856,7 +4861,7 @@
       <c r="A90">
         <v>44</v>
       </c>
-      <c r="B90" s="83">
+      <c r="B90" s="52">
         <v>4.2</v>
       </c>
     </row>
@@ -4864,7 +4869,7 @@
       <c r="A91">
         <v>44.5</v>
       </c>
-      <c r="B91" s="83">
+      <c r="B91" s="52">
         <v>4.3</v>
       </c>
     </row>
@@ -4872,7 +4877,7 @@
       <c r="A92">
         <v>45</v>
       </c>
-      <c r="B92" s="83">
+      <c r="B92" s="52">
         <v>4.3</v>
       </c>
     </row>
@@ -4880,7 +4885,7 @@
       <c r="A93">
         <v>45.5</v>
       </c>
-      <c r="B93" s="83">
+      <c r="B93" s="52">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -4888,7 +4893,7 @@
       <c r="A94">
         <v>46</v>
       </c>
-      <c r="B94" s="83">
+      <c r="B94" s="52">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -4896,7 +4901,7 @@
       <c r="A95">
         <v>46.5</v>
       </c>
-      <c r="B95" s="83">
+      <c r="B95" s="52">
         <v>4.5</v>
       </c>
     </row>
@@ -4904,7 +4909,7 @@
       <c r="A96">
         <v>47</v>
       </c>
-      <c r="B96" s="83">
+      <c r="B96" s="52">
         <v>4.5</v>
       </c>
     </row>
@@ -4912,7 +4917,7 @@
       <c r="A97">
         <v>47.5</v>
       </c>
-      <c r="B97" s="83">
+      <c r="B97" s="52">
         <v>4.5999999999999996</v>
       </c>
     </row>
@@ -4920,7 +4925,7 @@
       <c r="A98">
         <v>48</v>
       </c>
-      <c r="B98" s="83">
+      <c r="B98" s="52">
         <v>4.5999999999999996</v>
       </c>
     </row>
@@ -4928,7 +4933,7 @@
       <c r="A99">
         <v>48.5</v>
       </c>
-      <c r="B99" s="83">
+      <c r="B99" s="52">
         <v>4.7</v>
       </c>
     </row>
@@ -4936,7 +4941,7 @@
       <c r="A100">
         <v>49</v>
       </c>
-      <c r="B100" s="83">
+      <c r="B100" s="52">
         <v>4.8</v>
       </c>
     </row>
@@ -4944,7 +4949,7 @@
       <c r="A101">
         <v>49.5</v>
       </c>
-      <c r="B101" s="83">
+      <c r="B101" s="52">
         <v>4.8</v>
       </c>
     </row>
@@ -4952,7 +4957,7 @@
       <c r="A102">
         <v>50</v>
       </c>
-      <c r="B102" s="83">
+      <c r="B102" s="52">
         <v>4.9000000000000004</v>
       </c>
     </row>
@@ -4960,7 +4965,7 @@
       <c r="A103">
         <v>50.5</v>
       </c>
-      <c r="B103" s="83">
+      <c r="B103" s="52">
         <v>4.9000000000000004</v>
       </c>
     </row>
@@ -4968,7 +4973,7 @@
       <c r="A104">
         <v>51</v>
       </c>
-      <c r="B104" s="83">
+      <c r="B104" s="52">
         <v>5</v>
       </c>
     </row>
@@ -4976,7 +4981,7 @@
       <c r="A105">
         <v>51.5</v>
       </c>
-      <c r="B105" s="83">
+      <c r="B105" s="52">
         <v>5</v>
       </c>
     </row>
@@ -4984,7 +4989,7 @@
       <c r="A106">
         <v>52</v>
       </c>
-      <c r="B106" s="83">
+      <c r="B106" s="52">
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -4992,7 +4997,7 @@
       <c r="A107">
         <v>52.5</v>
       </c>
-      <c r="B107" s="83">
+      <c r="B107" s="52">
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -5000,7 +5005,7 @@
       <c r="A108">
         <v>53</v>
       </c>
-      <c r="B108" s="83">
+      <c r="B108" s="52">
         <v>5.2</v>
       </c>
     </row>
@@ -5008,7 +5013,7 @@
       <c r="A109">
         <v>53.5</v>
       </c>
-      <c r="B109" s="83">
+      <c r="B109" s="52">
         <v>5.2</v>
       </c>
     </row>
@@ -5016,7 +5021,7 @@
       <c r="A110">
         <v>54</v>
       </c>
-      <c r="B110" s="83">
+      <c r="B110" s="52">
         <v>5.3</v>
       </c>
     </row>
@@ -5024,7 +5029,7 @@
       <c r="A111">
         <v>54.5</v>
       </c>
-      <c r="B111" s="83">
+      <c r="B111" s="52">
         <v>5.3</v>
       </c>
     </row>
@@ -5032,7 +5037,7 @@
       <c r="A112">
         <v>55</v>
       </c>
-      <c r="B112" s="83">
+      <c r="B112" s="52">
         <v>5.4</v>
       </c>
     </row>
@@ -5040,7 +5045,7 @@
       <c r="A113">
         <v>55.5</v>
       </c>
-      <c r="B113" s="83">
+      <c r="B113" s="52">
         <v>5.4</v>
       </c>
     </row>
@@ -5048,7 +5053,7 @@
       <c r="A114">
         <v>56</v>
       </c>
-      <c r="B114" s="83">
+      <c r="B114" s="52">
         <v>5.5</v>
       </c>
     </row>
@@ -5056,7 +5061,7 @@
       <c r="A115">
         <v>56.5</v>
       </c>
-      <c r="B115" s="83">
+      <c r="B115" s="52">
         <v>5.6</v>
       </c>
     </row>
@@ -5064,7 +5069,7 @@
       <c r="A116">
         <v>57</v>
       </c>
-      <c r="B116" s="83">
+      <c r="B116" s="52">
         <v>5.6</v>
       </c>
     </row>
@@ -5072,7 +5077,7 @@
       <c r="A117">
         <v>57.5</v>
       </c>
-      <c r="B117" s="83">
+      <c r="B117" s="52">
         <v>5.7</v>
       </c>
     </row>
@@ -5080,7 +5085,7 @@
       <c r="A118">
         <v>58</v>
       </c>
-      <c r="B118" s="83">
+      <c r="B118" s="52">
         <v>5.7</v>
       </c>
     </row>
@@ -5088,7 +5093,7 @@
       <c r="A119">
         <v>58.5</v>
       </c>
-      <c r="B119" s="83">
+      <c r="B119" s="52">
         <v>5.8</v>
       </c>
     </row>
@@ -5096,7 +5101,7 @@
       <c r="A120">
         <v>59</v>
       </c>
-      <c r="B120" s="83">
+      <c r="B120" s="52">
         <v>5.8</v>
       </c>
     </row>
@@ -5104,7 +5109,7 @@
       <c r="A121">
         <v>59.5</v>
       </c>
-      <c r="B121" s="83">
+      <c r="B121" s="52">
         <v>5.9</v>
       </c>
     </row>
@@ -5112,7 +5117,7 @@
       <c r="A122">
         <v>60</v>
       </c>
-      <c r="B122" s="83">
+      <c r="B122" s="52">
         <v>5.9</v>
       </c>
     </row>
@@ -5120,7 +5125,7 @@
       <c r="A123">
         <v>60.5</v>
       </c>
-      <c r="B123" s="83">
+      <c r="B123" s="52">
         <v>6</v>
       </c>
     </row>
@@ -5128,7 +5133,7 @@
       <c r="A124">
         <v>61</v>
       </c>
-      <c r="B124" s="83">
+      <c r="B124" s="52">
         <v>6</v>
       </c>
     </row>
@@ -5136,7 +5141,7 @@
       <c r="A125">
         <v>61.5</v>
       </c>
-      <c r="B125" s="83">
+      <c r="B125" s="52">
         <v>6.1</v>
       </c>
     </row>
@@ -5144,7 +5149,7 @@
       <c r="A126">
         <v>62</v>
       </c>
-      <c r="B126" s="83">
+      <c r="B126" s="52">
         <v>6.1</v>
       </c>
     </row>
@@ -5152,7 +5157,7 @@
       <c r="A127">
         <v>62.5</v>
       </c>
-      <c r="B127" s="83">
+      <c r="B127" s="52">
         <v>6.2</v>
       </c>
     </row>
@@ -5160,7 +5165,7 @@
       <c r="A128">
         <v>63</v>
       </c>
-      <c r="B128" s="83">
+      <c r="B128" s="52">
         <v>6.3</v>
       </c>
     </row>
@@ -5168,7 +5173,7 @@
       <c r="A129">
         <v>63.5</v>
       </c>
-      <c r="B129" s="83">
+      <c r="B129" s="52">
         <v>6.3</v>
       </c>
     </row>
@@ -5176,7 +5181,7 @@
       <c r="A130">
         <v>64</v>
       </c>
-      <c r="B130" s="83">
+      <c r="B130" s="52">
         <v>6.4</v>
       </c>
     </row>
@@ -5184,7 +5189,7 @@
       <c r="A131">
         <v>64.5</v>
       </c>
-      <c r="B131" s="83">
+      <c r="B131" s="52">
         <v>6.4</v>
       </c>
     </row>
@@ -5192,7 +5197,7 @@
       <c r="A132">
         <v>65</v>
       </c>
-      <c r="B132" s="83">
+      <c r="B132" s="52">
         <v>6.5</v>
       </c>
     </row>
@@ -5200,7 +5205,7 @@
       <c r="A133">
         <v>65.5</v>
       </c>
-      <c r="B133" s="83">
+      <c r="B133" s="52">
         <v>6.5</v>
       </c>
     </row>
@@ -5208,7 +5213,7 @@
       <c r="A134">
         <v>66</v>
       </c>
-      <c r="B134" s="83">
+      <c r="B134" s="52">
         <v>6.6</v>
       </c>
     </row>
@@ -5216,7 +5221,7 @@
       <c r="A135">
         <v>66.5</v>
       </c>
-      <c r="B135" s="83">
+      <c r="B135" s="52">
         <v>6.6</v>
       </c>
     </row>
@@ -5224,7 +5229,7 @@
       <c r="A136">
         <v>67</v>
       </c>
-      <c r="B136" s="83">
+      <c r="B136" s="52">
         <v>6.7</v>
       </c>
     </row>
@@ -5232,7 +5237,7 @@
       <c r="A137">
         <v>67.5</v>
       </c>
-      <c r="B137" s="83">
+      <c r="B137" s="52">
         <v>6.7</v>
       </c>
     </row>
@@ -5240,7 +5245,7 @@
       <c r="A138">
         <v>68</v>
       </c>
-      <c r="B138" s="83">
+      <c r="B138" s="52">
         <v>6.8</v>
       </c>
     </row>
@@ -5248,7 +5253,7 @@
       <c r="A139">
         <v>68.5</v>
       </c>
-      <c r="B139" s="83">
+      <c r="B139" s="52">
         <v>6.8</v>
       </c>
     </row>
@@ -5256,7 +5261,7 @@
       <c r="A140">
         <v>69</v>
       </c>
-      <c r="B140" s="83">
+      <c r="B140" s="52">
         <v>6.9</v>
       </c>
     </row>
@@ -5264,7 +5269,7 @@
       <c r="A141">
         <v>69.5</v>
       </c>
-      <c r="B141" s="83">
+      <c r="B141" s="52">
         <v>6.9</v>
       </c>
     </row>
@@ -5272,7 +5277,7 @@
       <c r="A142">
         <v>70</v>
       </c>
-      <c r="B142" s="83">
+      <c r="B142" s="52">
         <v>7</v>
       </c>
     </row>
@@ -7560,7 +7565,7 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="83">
+      <c r="B2" s="52">
         <v>1</v>
       </c>
     </row>
@@ -7568,7 +7573,7 @@
       <c r="A3">
         <v>0.5</v>
       </c>
-      <c r="B3" s="83">
+      <c r="B3" s="52">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -7576,7 +7581,7 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="83">
+      <c r="B4" s="52">
         <v>1.2</v>
       </c>
     </row>
@@ -7584,7 +7589,7 @@
       <c r="A5">
         <v>1.5</v>
       </c>
-      <c r="B5" s="83">
+      <c r="B5" s="52">
         <v>1.3</v>
       </c>
     </row>
@@ -7592,7 +7597,7 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="83">
+      <c r="B6" s="52">
         <v>1.3</v>
       </c>
     </row>
@@ -7600,7 +7605,7 @@
       <c r="A7">
         <v>2.5</v>
       </c>
-      <c r="B7" s="83">
+      <c r="B7" s="52">
         <v>1.4</v>
       </c>
     </row>
@@ -7608,7 +7613,7 @@
       <c r="A8">
         <v>3</v>
       </c>
-      <c r="B8" s="83">
+      <c r="B8" s="52">
         <v>1.5</v>
       </c>
     </row>
@@ -7616,7 +7621,7 @@
       <c r="A9">
         <v>3.5</v>
       </c>
-      <c r="B9" s="83">
+      <c r="B9" s="52">
         <v>1.6</v>
       </c>
     </row>
@@ -7624,7 +7629,7 @@
       <c r="A10">
         <v>4</v>
       </c>
-      <c r="B10" s="83">
+      <c r="B10" s="52">
         <v>1.7</v>
       </c>
     </row>
@@ -7632,7 +7637,7 @@
       <c r="A11">
         <v>4.5</v>
       </c>
-      <c r="B11" s="83">
+      <c r="B11" s="52">
         <v>1.8</v>
       </c>
     </row>
@@ -7640,7 +7645,7 @@
       <c r="A12">
         <v>5</v>
       </c>
-      <c r="B12" s="83">
+      <c r="B12" s="52">
         <v>1.8</v>
       </c>
     </row>
@@ -7648,7 +7653,7 @@
       <c r="A13">
         <v>5.5</v>
       </c>
-      <c r="B13" s="83">
+      <c r="B13" s="52">
         <v>1.9</v>
       </c>
     </row>
@@ -7656,7 +7661,7 @@
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14" s="83">
+      <c r="B14" s="52">
         <v>2</v>
       </c>
     </row>
@@ -7664,7 +7669,7 @@
       <c r="A15">
         <v>6.5</v>
       </c>
-      <c r="B15" s="83">
+      <c r="B15" s="52">
         <v>2.1</v>
       </c>
     </row>
@@ -7672,7 +7677,7 @@
       <c r="A16">
         <v>7</v>
       </c>
-      <c r="B16" s="83">
+      <c r="B16" s="52">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -7680,7 +7685,7 @@
       <c r="A17">
         <v>7.5</v>
       </c>
-      <c r="B17" s="83">
+      <c r="B17" s="52">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -7688,7 +7693,7 @@
       <c r="A18">
         <v>8</v>
       </c>
-      <c r="B18" s="83">
+      <c r="B18" s="52">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -7696,7 +7701,7 @@
       <c r="A19">
         <v>8.5</v>
       </c>
-      <c r="B19" s="83">
+      <c r="B19" s="52">
         <v>2.4</v>
       </c>
     </row>
@@ -7704,7 +7709,7 @@
       <c r="A20">
         <v>9</v>
       </c>
-      <c r="B20" s="83">
+      <c r="B20" s="52">
         <v>2.5</v>
       </c>
     </row>
@@ -7712,7 +7717,7 @@
       <c r="A21">
         <v>9.5</v>
       </c>
-      <c r="B21" s="83">
+      <c r="B21" s="52">
         <v>2.6</v>
       </c>
     </row>
@@ -7720,7 +7725,7 @@
       <c r="A22">
         <v>10</v>
       </c>
-      <c r="B22" s="83">
+      <c r="B22" s="52">
         <v>2.7</v>
       </c>
     </row>
@@ -7728,7 +7733,7 @@
       <c r="A23">
         <v>10.5</v>
       </c>
-      <c r="B23" s="83">
+      <c r="B23" s="52">
         <v>2.8</v>
       </c>
     </row>
@@ -7736,7 +7741,7 @@
       <c r="A24">
         <v>11</v>
       </c>
-      <c r="B24" s="83">
+      <c r="B24" s="52">
         <v>2.8</v>
       </c>
     </row>
@@ -7744,7 +7749,7 @@
       <c r="A25">
         <v>11.5</v>
       </c>
-      <c r="B25" s="83">
+      <c r="B25" s="52">
         <v>2.9</v>
       </c>
     </row>
@@ -7752,7 +7757,7 @@
       <c r="A26">
         <v>12</v>
       </c>
-      <c r="B26" s="83">
+      <c r="B26" s="52">
         <v>3</v>
       </c>
     </row>
@@ -7760,7 +7765,7 @@
       <c r="A27">
         <v>12.5</v>
       </c>
-      <c r="B27" s="83">
+      <c r="B27" s="52">
         <v>3.1</v>
       </c>
     </row>
@@ -7768,7 +7773,7 @@
       <c r="A28">
         <v>13</v>
       </c>
-      <c r="B28" s="83">
+      <c r="B28" s="52">
         <v>3.2</v>
       </c>
     </row>
@@ -7776,7 +7781,7 @@
       <c r="A29">
         <v>13.5</v>
       </c>
-      <c r="B29" s="83">
+      <c r="B29" s="52">
         <v>3.3</v>
       </c>
     </row>
@@ -7784,7 +7789,7 @@
       <c r="A30">
         <v>14</v>
       </c>
-      <c r="B30" s="83">
+      <c r="B30" s="52">
         <v>3.3</v>
       </c>
     </row>
@@ -7792,7 +7797,7 @@
       <c r="A31">
         <v>14.5</v>
       </c>
-      <c r="B31" s="83">
+      <c r="B31" s="52">
         <v>3.4</v>
       </c>
     </row>
@@ -7800,7 +7805,7 @@
       <c r="A32">
         <v>15</v>
       </c>
-      <c r="B32" s="83">
+      <c r="B32" s="52">
         <v>3.5</v>
       </c>
     </row>
@@ -7808,7 +7813,7 @@
       <c r="A33">
         <v>15.5</v>
       </c>
-      <c r="B33" s="83">
+      <c r="B33" s="52">
         <v>3.6</v>
       </c>
     </row>
@@ -7816,7 +7821,7 @@
       <c r="A34">
         <v>16</v>
       </c>
-      <c r="B34" s="83">
+      <c r="B34" s="52">
         <v>3.7</v>
       </c>
     </row>
@@ -7824,7 +7829,7 @@
       <c r="A35">
         <v>16.5</v>
       </c>
-      <c r="B35" s="83">
+      <c r="B35" s="52">
         <v>3.8</v>
       </c>
     </row>
@@ -7832,7 +7837,7 @@
       <c r="A36">
         <v>17</v>
       </c>
-      <c r="B36" s="83">
+      <c r="B36" s="52">
         <v>3.8</v>
       </c>
     </row>
@@ -7840,7 +7845,7 @@
       <c r="A37">
         <v>17.5</v>
       </c>
-      <c r="B37" s="83">
+      <c r="B37" s="52">
         <v>3.9</v>
       </c>
     </row>
@@ -7848,7 +7853,7 @@
       <c r="A38">
         <v>18</v>
       </c>
-      <c r="B38" s="83">
+      <c r="B38" s="52">
         <v>4</v>
       </c>
     </row>
@@ -7856,7 +7861,7 @@
       <c r="A39">
         <v>18.5</v>
       </c>
-      <c r="B39" s="83">
+      <c r="B39" s="52">
         <v>4.0999999999999996</v>
       </c>
     </row>
@@ -7864,7 +7869,7 @@
       <c r="A40">
         <v>19</v>
       </c>
-      <c r="B40" s="83">
+      <c r="B40" s="52">
         <v>4.3</v>
       </c>
     </row>
@@ -7872,7 +7877,7 @@
       <c r="A41">
         <v>19.5</v>
       </c>
-      <c r="B41" s="83">
+      <c r="B41" s="52">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -7880,7 +7885,7 @@
       <c r="A42">
         <v>20</v>
       </c>
-      <c r="B42" s="83">
+      <c r="B42" s="52">
         <v>4.5</v>
       </c>
     </row>
@@ -7888,7 +7893,7 @@
       <c r="A43">
         <v>20.5</v>
       </c>
-      <c r="B43" s="83">
+      <c r="B43" s="52">
         <v>4.5999999999999996</v>
       </c>
     </row>
@@ -7896,7 +7901,7 @@
       <c r="A44">
         <v>21</v>
       </c>
-      <c r="B44" s="83">
+      <c r="B44" s="52">
         <v>4.8</v>
       </c>
     </row>
@@ -7904,7 +7909,7 @@
       <c r="A45">
         <v>21.5</v>
       </c>
-      <c r="B45" s="83">
+      <c r="B45" s="52">
         <v>4.9000000000000004</v>
       </c>
     </row>
@@ -7912,7 +7917,7 @@
       <c r="A46">
         <v>22</v>
       </c>
-      <c r="B46" s="83">
+      <c r="B46" s="52">
         <v>5</v>
       </c>
     </row>
@@ -7920,7 +7925,7 @@
       <c r="A47">
         <v>22.5</v>
       </c>
-      <c r="B47" s="83">
+      <c r="B47" s="52">
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -7928,7 +7933,7 @@
       <c r="A48">
         <v>23</v>
       </c>
-      <c r="B48" s="83">
+      <c r="B48" s="52">
         <v>5.3</v>
       </c>
     </row>
@@ -7936,7 +7941,7 @@
       <c r="A49">
         <v>23.5</v>
       </c>
-      <c r="B49" s="83">
+      <c r="B49" s="52">
         <v>5.4</v>
       </c>
     </row>
@@ -7944,7 +7949,7 @@
       <c r="A50">
         <v>24</v>
       </c>
-      <c r="B50" s="83">
+      <c r="B50" s="52">
         <v>5.5</v>
       </c>
     </row>
@@ -7952,7 +7957,7 @@
       <c r="A51">
         <v>24.5</v>
       </c>
-      <c r="B51" s="83">
+      <c r="B51" s="52">
         <v>5.6</v>
       </c>
     </row>
@@ -7960,7 +7965,7 @@
       <c r="A52">
         <v>25</v>
       </c>
-      <c r="B52" s="83">
+      <c r="B52" s="52">
         <v>5.8</v>
       </c>
     </row>
@@ -7968,7 +7973,7 @@
       <c r="A53">
         <v>25.5</v>
       </c>
-      <c r="B53" s="83">
+      <c r="B53" s="52">
         <v>5.9</v>
       </c>
     </row>
@@ -7976,7 +7981,7 @@
       <c r="A54">
         <v>26</v>
       </c>
-      <c r="B54" s="83">
+      <c r="B54" s="52">
         <v>6</v>
       </c>
     </row>
@@ -7984,7 +7989,7 @@
       <c r="A55">
         <v>26.5</v>
       </c>
-      <c r="B55" s="83">
+      <c r="B55" s="52">
         <v>6.1</v>
       </c>
     </row>
@@ -7992,7 +7997,7 @@
       <c r="A56">
         <v>27</v>
       </c>
-      <c r="B56" s="83">
+      <c r="B56" s="52">
         <v>6.3</v>
       </c>
     </row>
@@ -8000,7 +8005,7 @@
       <c r="A57">
         <v>27.5</v>
       </c>
-      <c r="B57" s="83">
+      <c r="B57" s="52">
         <v>6.4</v>
       </c>
     </row>
@@ -8008,7 +8013,7 @@
       <c r="A58">
         <v>28</v>
       </c>
-      <c r="B58" s="83">
+      <c r="B58" s="52">
         <v>6.5</v>
       </c>
     </row>
@@ -8016,7 +8021,7 @@
       <c r="A59">
         <v>28.5</v>
       </c>
-      <c r="B59" s="83">
+      <c r="B59" s="52">
         <v>6.6</v>
       </c>
     </row>
@@ -8024,7 +8029,7 @@
       <c r="A60">
         <v>29</v>
       </c>
-      <c r="B60" s="83">
+      <c r="B60" s="52">
         <v>6.8</v>
       </c>
     </row>
@@ -8032,7 +8037,7 @@
       <c r="A61">
         <v>29.5</v>
       </c>
-      <c r="B61" s="83">
+      <c r="B61" s="52">
         <v>6.9</v>
       </c>
     </row>
@@ -8040,7 +8045,7 @@
       <c r="A62">
         <v>30</v>
       </c>
-      <c r="B62" s="83">
+      <c r="B62" s="52">
         <v>7</v>
       </c>
     </row>
@@ -9002,7 +9007,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -9013,7 +9018,7 @@
       <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="75"/>
+      <c r="A2" s="83"/>
       <c r="B2" s="10" t="s">
         <v>7</v>
       </c>

</xml_diff>